<commit_message>
Added method to display brand values as core entities
</commit_message>
<xml_diff>
--- a/datageneration/data/Primary_Keys_filtered10.xlsx
+++ b/datageneration/data/Primary_Keys_filtered10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deutschewelle.sharepoint.com/teams/GR-GR-ReCo-KID2/Freigegebene Dokumente/General/03_Ongoing Work/03C_MS_Spot - ongoing/03Cc_Development/Key-Value Pairs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1973C027-50CC-45C2-BF9A-783B971E00D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEE9AB39-29C9-4C86-8D78-4577D7C562ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35920" yWindow="-2460" windowWidth="35840" windowHeight="21100" xr2:uid="{0ED01DE8-A235-1045-8C96-52557544134F}"/>
   </bookViews>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="1225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2125" uniqueCount="1225">
   <si>
     <t>index</t>
   </si>
@@ -2691,7 +2691,7 @@
     <t>addr:street~***any***</t>
   </si>
   <si>
-    <t>name, brand, brand name</t>
+    <t>name|brand|brand name</t>
   </si>
   <si>
     <t>name~***example***, brand~***example***</t>
@@ -4187,8 +4187,8 @@
   <dimension ref="A1:H605"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B532" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F546" sqref="F546"/>
+      <pane ySplit="1" topLeftCell="A574" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C593" sqref="C593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -9068,6 +9068,9 @@
       <c r="B308" s="2" t="s">
         <v>631</v>
       </c>
+      <c r="C308" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D308" s="6" t="s">
         <v>3</v>
       </c>
@@ -9334,6 +9337,9 @@
       <c r="B327" s="2" t="s">
         <v>669</v>
       </c>
+      <c r="C327" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D327" s="6" t="s">
         <v>9</v>
       </c>
@@ -9348,6 +9354,9 @@
       <c r="B328" s="2" t="s">
         <v>671</v>
       </c>
+      <c r="C328" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D328" s="6" t="s">
         <v>9</v>
       </c>
@@ -9362,6 +9371,9 @@
       <c r="B329" s="2" t="s">
         <v>673</v>
       </c>
+      <c r="C329" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D329" s="6" t="s">
         <v>9</v>
       </c>
@@ -9376,6 +9388,9 @@
       <c r="B330" s="2" t="s">
         <v>675</v>
       </c>
+      <c r="C330" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D330" s="6" t="s">
         <v>9</v>
       </c>
@@ -9390,6 +9405,9 @@
       <c r="B331" s="2" t="s">
         <v>677</v>
       </c>
+      <c r="C331" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D331" s="6" t="s">
         <v>9</v>
       </c>
@@ -9404,6 +9422,9 @@
       <c r="B332" s="2" t="s">
         <v>679</v>
       </c>
+      <c r="C332" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D332" s="6" t="s">
         <v>9</v>
       </c>
@@ -9418,6 +9439,9 @@
       <c r="B333" s="2" t="s">
         <v>681</v>
       </c>
+      <c r="C333" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D333" s="6" t="s">
         <v>9</v>
       </c>
@@ -9432,6 +9456,9 @@
       <c r="B334" s="2" t="s">
         <v>683</v>
       </c>
+      <c r="C334" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D334" s="6" t="s">
         <v>9</v>
       </c>
@@ -9446,6 +9473,9 @@
       <c r="B335" s="2" t="s">
         <v>685</v>
       </c>
+      <c r="C335" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D335" s="6" t="s">
         <v>9</v>
       </c>
@@ -9460,6 +9490,9 @@
       <c r="B336" s="2" t="s">
         <v>687</v>
       </c>
+      <c r="C336" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D336" s="6" t="s">
         <v>3</v>
       </c>
@@ -9474,6 +9507,9 @@
       <c r="B337" s="2" t="s">
         <v>689</v>
       </c>
+      <c r="C337" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D337" s="6" t="s">
         <v>9</v>
       </c>
@@ -9488,6 +9524,9 @@
       <c r="B338" s="2" t="s">
         <v>691</v>
       </c>
+      <c r="C338" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D338" s="6" t="s">
         <v>9</v>
       </c>
@@ -9502,6 +9541,9 @@
       <c r="B339" s="2" t="s">
         <v>693</v>
       </c>
+      <c r="C339" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D339" s="6" t="s">
         <v>9</v>
       </c>
@@ -9513,6 +9555,9 @@
       <c r="B340" s="2" t="s">
         <v>695</v>
       </c>
+      <c r="C340" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D340" s="6" t="s">
         <v>9</v>
       </c>
@@ -9527,6 +9572,9 @@
       <c r="B341" s="2" t="s">
         <v>697</v>
       </c>
+      <c r="C341" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D341" s="6" t="s">
         <v>3</v>
       </c>
@@ -9541,6 +9589,9 @@
       <c r="B342" s="2" t="s">
         <v>699</v>
       </c>
+      <c r="C342" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D342" s="6" t="s">
         <v>3</v>
       </c>
@@ -9569,6 +9620,9 @@
       <c r="B344" s="2" t="s">
         <v>703</v>
       </c>
+      <c r="C344" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D344" s="6" t="s">
         <v>36</v>
       </c>
@@ -9583,6 +9637,9 @@
       <c r="B345" s="2" t="s">
         <v>705</v>
       </c>
+      <c r="C345" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D345" s="6" t="s">
         <v>9</v>
       </c>
@@ -9681,6 +9738,9 @@
       <c r="B352" s="2" t="s">
         <v>719</v>
       </c>
+      <c r="C352" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D352" s="6" t="s">
         <v>3</v>
       </c>
@@ -9695,6 +9755,9 @@
       <c r="B353" s="2" t="s">
         <v>721</v>
       </c>
+      <c r="C353" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D353" s="6" t="s">
         <v>3</v>
       </c>
@@ -10154,6 +10217,9 @@
       <c r="B386" s="2" t="s">
         <v>787</v>
       </c>
+      <c r="C386" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D386" s="6" t="s">
         <v>9</v>
       </c>
@@ -10168,6 +10234,9 @@
       <c r="B387" s="2" t="s">
         <v>789</v>
       </c>
+      <c r="C387" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D387" s="6" t="s">
         <v>9</v>
       </c>
@@ -10182,6 +10251,9 @@
       <c r="B388" s="2" t="s">
         <v>791</v>
       </c>
+      <c r="C388" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D388" s="6" t="s">
         <v>9</v>
       </c>
@@ -10243,6 +10315,9 @@
       <c r="B393" s="2" t="s">
         <v>801</v>
       </c>
+      <c r="C393" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D393" s="6" t="s">
         <v>9</v>
       </c>
@@ -10257,6 +10332,9 @@
       <c r="B394" s="2" t="s">
         <v>803</v>
       </c>
+      <c r="C394" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D394" s="6" t="s">
         <v>9</v>
       </c>
@@ -10271,6 +10349,9 @@
       <c r="B395" s="2" t="s">
         <v>805</v>
       </c>
+      <c r="C395" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D395" s="6" t="s">
         <v>9</v>
       </c>
@@ -10285,6 +10366,9 @@
       <c r="B396" s="2" t="s">
         <v>807</v>
       </c>
+      <c r="C396" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D396" s="6" t="s">
         <v>9</v>
       </c>
@@ -10313,6 +10397,9 @@
       <c r="B398" s="2" t="s">
         <v>811</v>
       </c>
+      <c r="C398" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D398" s="6" t="s">
         <v>9</v>
       </c>
@@ -10327,6 +10414,9 @@
       <c r="B399" s="2" t="s">
         <v>813</v>
       </c>
+      <c r="C399" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D399" s="6" t="s">
         <v>9</v>
       </c>
@@ -10341,6 +10431,9 @@
       <c r="B400" s="2" t="s">
         <v>815</v>
       </c>
+      <c r="C400" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D400" s="6" t="s">
         <v>9</v>
       </c>
@@ -10397,6 +10490,9 @@
       <c r="B404" s="2" t="s">
         <v>823</v>
       </c>
+      <c r="C404" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D404" s="6" t="s">
         <v>3</v>
       </c>
@@ -10439,6 +10535,9 @@
       <c r="B407" s="2" t="s">
         <v>829</v>
       </c>
+      <c r="C407" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D407" s="6" t="s">
         <v>3</v>
       </c>
@@ -10453,6 +10552,9 @@
       <c r="B408" s="2" t="s">
         <v>831</v>
       </c>
+      <c r="C408" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D408" s="6" t="s">
         <v>9</v>
       </c>
@@ -10467,6 +10569,9 @@
       <c r="B409" s="2" t="s">
         <v>833</v>
       </c>
+      <c r="C409" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D409" s="6" t="s">
         <v>9</v>
       </c>
@@ -10509,6 +10614,9 @@
       <c r="B412" s="2" t="s">
         <v>839</v>
       </c>
+      <c r="C412" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D412" s="6" t="s">
         <v>9</v>
       </c>
@@ -10523,6 +10631,9 @@
       <c r="B413" s="2" t="s">
         <v>841</v>
       </c>
+      <c r="C413" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D413" s="6" t="s">
         <v>9</v>
       </c>
@@ -10537,6 +10648,9 @@
       <c r="B414" s="2" t="s">
         <v>843</v>
       </c>
+      <c r="C414" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D414" s="6" t="s">
         <v>9</v>
       </c>
@@ -10551,6 +10665,9 @@
       <c r="B415" s="2" t="s">
         <v>845</v>
       </c>
+      <c r="C415" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D415" s="6" t="s">
         <v>9</v>
       </c>
@@ -10565,6 +10682,9 @@
       <c r="B416" s="2" t="s">
         <v>847</v>
       </c>
+      <c r="C416" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D416" s="6" t="s">
         <v>9</v>
       </c>
@@ -10579,6 +10699,9 @@
       <c r="B417" s="2" t="s">
         <v>849</v>
       </c>
+      <c r="C417" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D417" s="6" t="s">
         <v>9</v>
       </c>
@@ -10635,6 +10758,9 @@
       <c r="B421" s="2" t="s">
         <v>857</v>
       </c>
+      <c r="C421" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D421" s="6" t="s">
         <v>9</v>
       </c>
@@ -10663,6 +10789,9 @@
       <c r="B423" s="2" t="s">
         <v>861</v>
       </c>
+      <c r="C423" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D423" s="6" t="s">
         <v>9</v>
       </c>
@@ -10761,6 +10890,9 @@
       <c r="B430" s="2" t="s">
         <v>875</v>
       </c>
+      <c r="C430" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D430" s="6" t="s">
         <v>9</v>
       </c>
@@ -10786,6 +10918,9 @@
       <c r="B432" s="2" t="s">
         <v>879</v>
       </c>
+      <c r="C432" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D432" s="6" t="s">
         <v>9</v>
       </c>
@@ -10842,6 +10977,9 @@
       <c r="B436" s="2" t="s">
         <v>887</v>
       </c>
+      <c r="C436" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D436" s="6" t="s">
         <v>3</v>
       </c>
@@ -11051,6 +11189,9 @@
       <c r="B452" s="2" t="s">
         <v>917</v>
       </c>
+      <c r="C452" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D452" s="6" t="s">
         <v>9</v>
       </c>
@@ -11065,6 +11206,9 @@
       <c r="B453" s="2" t="s">
         <v>919</v>
       </c>
+      <c r="C453" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D453" s="6" t="s">
         <v>9</v>
       </c>
@@ -11079,6 +11223,9 @@
       <c r="B454" s="2" t="s">
         <v>921</v>
       </c>
+      <c r="C454" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D454" s="6" t="s">
         <v>9</v>
       </c>
@@ -11145,6 +11292,9 @@
       <c r="B460" s="2" t="s">
         <v>933</v>
       </c>
+      <c r="C460" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D460" s="6" t="s">
         <v>9</v>
       </c>
@@ -11156,6 +11306,9 @@
       <c r="B461" s="2" t="s">
         <v>935</v>
       </c>
+      <c r="C461" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D461" s="6" t="s">
         <v>9</v>
       </c>
@@ -11167,6 +11320,9 @@
       <c r="B462" s="2" t="s">
         <v>937</v>
       </c>
+      <c r="C462" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D462" s="6" t="s">
         <v>9</v>
       </c>
@@ -11299,6 +11455,9 @@
       <c r="B474" s="2" t="s">
         <v>961</v>
       </c>
+      <c r="C474" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D474" s="6" t="s">
         <v>3</v>
       </c>
@@ -11464,6 +11623,9 @@
       <c r="B489" s="2" t="s">
         <v>991</v>
       </c>
+      <c r="C489" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D489" s="6" t="s">
         <v>9</v>
       </c>
@@ -11486,6 +11648,9 @@
       <c r="B491" s="2" t="s">
         <v>995</v>
       </c>
+      <c r="C491" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D491" s="6" t="s">
         <v>9</v>
       </c>
@@ -11508,6 +11673,9 @@
       <c r="B493" s="2" t="s">
         <v>999</v>
       </c>
+      <c r="C493" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D493" s="6" t="s">
         <v>9</v>
       </c>
@@ -11519,6 +11687,9 @@
       <c r="B494" s="2" t="s">
         <v>1001</v>
       </c>
+      <c r="C494" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D494" s="6" t="s">
         <v>9</v>
       </c>
@@ -11530,6 +11701,9 @@
       <c r="B495" s="2" t="s">
         <v>1003</v>
       </c>
+      <c r="C495" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D495" s="6" t="s">
         <v>9</v>
       </c>
@@ -11541,6 +11715,9 @@
       <c r="B496" s="2" t="s">
         <v>1005</v>
       </c>
+      <c r="C496" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D496" s="6" t="s">
         <v>9</v>
       </c>
@@ -11552,6 +11729,9 @@
       <c r="B497" s="2" t="s">
         <v>1007</v>
       </c>
+      <c r="C497" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D497" s="6" t="s">
         <v>9</v>
       </c>
@@ -11563,6 +11743,9 @@
       <c r="B498" s="2" t="s">
         <v>1009</v>
       </c>
+      <c r="C498" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D498" s="6" t="s">
         <v>9</v>
       </c>
@@ -11574,6 +11757,9 @@
       <c r="B499" s="2" t="s">
         <v>1011</v>
       </c>
+      <c r="C499" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D499" s="6" t="s">
         <v>9</v>
       </c>
@@ -11585,6 +11771,9 @@
       <c r="B500" s="2" t="s">
         <v>1013</v>
       </c>
+      <c r="C500" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D500" s="6" t="s">
         <v>9</v>
       </c>
@@ -11596,6 +11785,9 @@
       <c r="B501" s="2" t="s">
         <v>1015</v>
       </c>
+      <c r="C501" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D501" s="6" t="s">
         <v>9</v>
       </c>
@@ -11607,6 +11799,9 @@
       <c r="B502" s="2" t="s">
         <v>1017</v>
       </c>
+      <c r="C502" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D502" s="6" t="s">
         <v>9</v>
       </c>
@@ -11618,6 +11813,9 @@
       <c r="B503" s="2" t="s">
         <v>1019</v>
       </c>
+      <c r="C503" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D503" s="6" t="s">
         <v>9</v>
       </c>
@@ -11629,6 +11827,9 @@
       <c r="B504" s="2" t="s">
         <v>1021</v>
       </c>
+      <c r="C504" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D504" s="6" t="s">
         <v>9</v>
       </c>
@@ -11640,6 +11841,9 @@
       <c r="B505" s="2" t="s">
         <v>1023</v>
       </c>
+      <c r="C505" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D505" s="6" t="s">
         <v>9</v>
       </c>
@@ -11651,6 +11855,9 @@
       <c r="B506" s="2" t="s">
         <v>1025</v>
       </c>
+      <c r="C506" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D506" s="6" t="s">
         <v>9</v>
       </c>
@@ -11662,6 +11869,9 @@
       <c r="B507" s="2" t="s">
         <v>1027</v>
       </c>
+      <c r="C507" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D507" s="6" t="s">
         <v>9</v>
       </c>
@@ -11673,6 +11883,9 @@
       <c r="B508" s="2" t="s">
         <v>1029</v>
       </c>
+      <c r="C508" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D508" s="6" t="s">
         <v>9</v>
       </c>
@@ -11684,6 +11897,9 @@
       <c r="B509" s="2" t="s">
         <v>1031</v>
       </c>
+      <c r="C509" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D509" s="6" t="s">
         <v>9</v>
       </c>
@@ -11695,6 +11911,9 @@
       <c r="B510" s="2" t="s">
         <v>1033</v>
       </c>
+      <c r="C510" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D510" s="6" t="s">
         <v>9</v>
       </c>
@@ -11706,6 +11925,9 @@
       <c r="B511" s="2" t="s">
         <v>1035</v>
       </c>
+      <c r="C511" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D511" s="6" t="s">
         <v>9</v>
       </c>
@@ -11717,6 +11939,9 @@
       <c r="B512" s="2" t="s">
         <v>1037</v>
       </c>
+      <c r="C512" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D512" s="6" t="s">
         <v>9</v>
       </c>
@@ -11728,6 +11953,9 @@
       <c r="B513" s="2" t="s">
         <v>1039</v>
       </c>
+      <c r="C513" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D513" s="6" t="s">
         <v>9</v>
       </c>
@@ -11739,6 +11967,9 @@
       <c r="B514" s="2" t="s">
         <v>1041</v>
       </c>
+      <c r="C514" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D514" s="6" t="s">
         <v>9</v>
       </c>
@@ -11750,6 +11981,9 @@
       <c r="B515" s="2" t="s">
         <v>1043</v>
       </c>
+      <c r="C515" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D515" s="6" t="s">
         <v>9</v>
       </c>
@@ -11761,6 +11995,9 @@
       <c r="B516" s="2" t="s">
         <v>1045</v>
       </c>
+      <c r="C516" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D516" s="6" t="s">
         <v>9</v>
       </c>
@@ -11772,6 +12009,9 @@
       <c r="B517" s="2" t="s">
         <v>1047</v>
       </c>
+      <c r="C517" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D517" s="6" t="s">
         <v>9</v>
       </c>
@@ -11783,6 +12023,9 @@
       <c r="B518" s="2" t="s">
         <v>1049</v>
       </c>
+      <c r="C518" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D518" s="6" t="s">
         <v>9</v>
       </c>
@@ -11794,6 +12037,9 @@
       <c r="B519" s="2" t="s">
         <v>1051</v>
       </c>
+      <c r="C519" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D519" s="6" t="s">
         <v>9</v>
       </c>
@@ -11805,6 +12051,9 @@
       <c r="B520" s="2" t="s">
         <v>1053</v>
       </c>
+      <c r="C520" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D520" s="6" t="s">
         <v>9</v>
       </c>
@@ -11816,6 +12065,9 @@
       <c r="B521" s="2" t="s">
         <v>1055</v>
       </c>
+      <c r="C521" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D521" s="6" t="s">
         <v>9</v>
       </c>
@@ -11849,6 +12101,9 @@
       <c r="B524" s="2" t="s">
         <v>1061</v>
       </c>
+      <c r="C524" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D524" s="6" t="s">
         <v>9</v>
       </c>
@@ -11860,6 +12115,9 @@
       <c r="B525" s="2" t="s">
         <v>1063</v>
       </c>
+      <c r="C525" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D525" s="6" t="s">
         <v>3</v>
       </c>
@@ -11871,6 +12129,9 @@
       <c r="B526" s="2" t="s">
         <v>1065</v>
       </c>
+      <c r="C526" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D526" s="6" t="s">
         <v>3</v>
       </c>
@@ -11882,6 +12143,9 @@
       <c r="B527" s="2" t="s">
         <v>1067</v>
       </c>
+      <c r="C527" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D527" s="6" t="s">
         <v>3</v>
       </c>
@@ -11904,6 +12168,9 @@
       <c r="B529" s="2" t="s">
         <v>1071</v>
       </c>
+      <c r="C529" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D529" s="6" t="s">
         <v>9</v>
       </c>
@@ -11981,6 +12248,9 @@
       <c r="B536" s="2" t="s">
         <v>1085</v>
       </c>
+      <c r="C536" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D536" s="6" t="s">
         <v>36</v>
       </c>
@@ -12003,6 +12273,9 @@
       <c r="B538" s="2" t="s">
         <v>1089</v>
       </c>
+      <c r="C538" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D538" s="6" t="s">
         <v>3</v>
       </c>
@@ -12017,6 +12290,9 @@
       <c r="B539" s="2" t="s">
         <v>1091</v>
       </c>
+      <c r="C539" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D539" s="6" t="s">
         <v>9</v>
       </c>
@@ -12053,6 +12329,9 @@
       <c r="B542" s="2" t="s">
         <v>1097</v>
       </c>
+      <c r="C542" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D542" s="6" t="s">
         <v>9</v>
       </c>
@@ -12067,6 +12346,9 @@
       <c r="B543" s="2" t="s">
         <v>1099</v>
       </c>
+      <c r="C543" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D543" s="6" t="s">
         <v>9</v>
       </c>
@@ -12081,6 +12363,9 @@
       <c r="B544" s="2" t="s">
         <v>1101</v>
       </c>
+      <c r="C544" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D544" s="6" t="s">
         <v>9</v>
       </c>
@@ -12095,6 +12380,9 @@
       <c r="B545" s="2" t="s">
         <v>1103</v>
       </c>
+      <c r="C545" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D545" s="6" t="s">
         <v>9</v>
       </c>
@@ -12109,6 +12397,9 @@
       <c r="B546" s="2" t="s">
         <v>1105</v>
       </c>
+      <c r="C546" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D546" s="6" t="s">
         <v>9</v>
       </c>
@@ -12123,6 +12414,9 @@
       <c r="B547" s="2" t="s">
         <v>1107</v>
       </c>
+      <c r="C547" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D547" s="6" t="s">
         <v>9</v>
       </c>
@@ -12134,6 +12428,9 @@
       <c r="B548" s="2" t="s">
         <v>1109</v>
       </c>
+      <c r="C548" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D548" s="6" t="s">
         <v>9</v>
       </c>
@@ -12148,6 +12445,9 @@
       <c r="B549" s="2" t="s">
         <v>1111</v>
       </c>
+      <c r="C549" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D549" s="6" t="s">
         <v>9</v>
       </c>
@@ -12162,6 +12462,9 @@
       <c r="B550" s="2" t="s">
         <v>1113</v>
       </c>
+      <c r="C550" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D550" s="6" t="s">
         <v>9</v>
       </c>
@@ -12176,6 +12479,9 @@
       <c r="B551" s="2" t="s">
         <v>1115</v>
       </c>
+      <c r="C551" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D551" s="6" t="s">
         <v>9</v>
       </c>
@@ -12190,6 +12496,9 @@
       <c r="B552" s="2" t="s">
         <v>1117</v>
       </c>
+      <c r="C552" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D552" s="6" t="s">
         <v>9</v>
       </c>
@@ -12204,6 +12513,9 @@
       <c r="B553" s="2" t="s">
         <v>1119</v>
       </c>
+      <c r="C553" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D553" s="6" t="s">
         <v>9</v>
       </c>
@@ -12358,6 +12670,9 @@
       <c r="B567" s="2" t="s">
         <v>1147</v>
       </c>
+      <c r="C567" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D567" s="6" t="s">
         <v>9</v>
       </c>
@@ -12479,6 +12794,9 @@
       <c r="B578" s="2" t="s">
         <v>1169</v>
       </c>
+      <c r="C578" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D578" s="6" t="s">
         <v>9</v>
       </c>
@@ -12490,6 +12808,9 @@
       <c r="B579" s="2" t="s">
         <v>1171</v>
       </c>
+      <c r="C579" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D579" s="6" t="s">
         <v>9</v>
       </c>
@@ -12512,6 +12833,9 @@
       <c r="B581" s="2" t="s">
         <v>1175</v>
       </c>
+      <c r="C581" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D581" s="6" t="s">
         <v>9</v>
       </c>
@@ -12523,6 +12847,9 @@
       <c r="B582" s="2" t="s">
         <v>1177</v>
       </c>
+      <c r="C582" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D582" s="6" t="s">
         <v>9</v>
       </c>
@@ -12534,6 +12861,9 @@
       <c r="B583" s="2" t="s">
         <v>1179</v>
       </c>
+      <c r="C583" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D583" s="6" t="s">
         <v>9</v>
       </c>
@@ -12567,6 +12897,9 @@
       <c r="B586" s="2" t="s">
         <v>1185</v>
       </c>
+      <c r="C586" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D586" s="6" t="s">
         <v>9</v>
       </c>
@@ -12602,6 +12935,9 @@
       <c r="B589" s="2" t="s">
         <v>1191</v>
       </c>
+      <c r="C589" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D589" s="6" t="s">
         <v>3</v>
       </c>
@@ -12613,6 +12949,9 @@
       <c r="B590" s="2" t="s">
         <v>1193</v>
       </c>
+      <c r="C590" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D590" s="6" t="s">
         <v>3</v>
       </c>
@@ -12623,6 +12962,9 @@
     <row r="591" spans="2:8" ht="15.75" customHeight="1">
       <c r="B591" s="2" t="s">
         <v>1195</v>
+      </c>
+      <c r="C591" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D591" s="6" t="s">
         <v>9</v>
@@ -12792,15 +13134,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="fef4af80-67d0-434d-aa7c-17eed15b0840">
@@ -12811,7 +13144,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BB17A56B5CDE7946ADE40FE50F9E0E05" ma:contentTypeVersion="18" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c12e4e740a918a7fed87ba9ba111f97c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d852b27-1d95-4577-ac49-0d344a1f93d0" xmlns:ns3="fef4af80-67d0-434d-aa7c-17eed15b0840" xmlns:ns4="69e77a95-4add-417d-ac50-c09752e64638" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e87260b9d5c1107f3f51cd8889399417" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6d852b27-1d95-4577-ac49-0d344a1f93d0"/>
@@ -13071,16 +13404,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E49D155-2C11-4885-ACD3-E6D3BF89105E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2787CFFA-3460-4A04-BA0A-9FECDEAA6229}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2787CFFA-3460-4A04-BA0A-9FECDEAA6229}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB476E3C-1092-486A-9BFE-5C9EC71BF137}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB476E3C-1092-486A-9BFE-5C9EC71BF137}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E49D155-2C11-4885-ACD3-E6D3BF89105E}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Removed "contains_within_radius" relation, prompt improvements
</commit_message>
<xml_diff>
--- a/datageneration/data/Primary_Keys_filtered10.xlsx
+++ b/datageneration/data/Primary_Keys_filtered10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27706"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deutschewelle.sharepoint.com/teams/GR-GR-ReCo-KID2/Freigegebene Dokumente/General/03_Ongoing Work/03C_MS_Spot - ongoing/03Cc_Development/Key-Value Pairs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6CE688C-764D-4C1A-AE25-99E98A8FE52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7270F832-46F4-47EA-9684-37B71232D3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35920" yWindow="-2460" windowWidth="35840" windowHeight="21100" xr2:uid="{0ED01DE8-A235-1045-8C96-52557544134F}"/>
   </bookViews>
@@ -543,7 +543,7 @@
     <t>amenity=childcare, amenity=kindergarten, building=kindergarten</t>
   </si>
   <si>
-    <t>clock|public clock| time| metronome| calendar| timer</t>
+    <t>public clock</t>
   </si>
   <si>
     <t>amenity=clock</t>
@@ -3375,7 +3375,7 @@
     <t>religion=***example***</t>
   </si>
   <si>
-    <t>catholic|roman catholic|sunni|baptist|lutheran|orthodox|anglican|protestant|methodist|russian orthodox|greek orthodox|jehovahs|evangelical|pentecostal|presbyterian|mormon|shia</t>
+    <t>denomination</t>
   </si>
   <si>
     <t>denomination=***example***</t>
@@ -4187,8 +4187,8 @@
   <dimension ref="A1:H605"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A574" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C593" sqref="C593"/>
+      <pane ySplit="1" topLeftCell="B522" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B541" sqref="B541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -13134,15 +13134,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="fef4af80-67d0-434d-aa7c-17eed15b0840">
@@ -13153,9 +13144,9 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BB17A56B5CDE7946ADE40FE50F9E0E05" ma:contentTypeVersion="18" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c12e4e740a918a7fed87ba9ba111f97c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d852b27-1d95-4577-ac49-0d344a1f93d0" xmlns:ns3="fef4af80-67d0-434d-aa7c-17eed15b0840" xmlns:ns4="69e77a95-4add-417d-ac50-c09752e64638" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e87260b9d5c1107f3f51cd8889399417" ns2:_="" ns3:_="" ns4:_="">
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB17A56B5CDE7946ADE40FE50F9E0E05" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1ef8fdae22ea8efa5f8e6ba78f2f5d7">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d852b27-1d95-4577-ac49-0d344a1f93d0" xmlns:ns3="fef4af80-67d0-434d-aa7c-17eed15b0840" xmlns:ns4="69e77a95-4add-417d-ac50-c09752e64638" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a57007e7f6e174e2eadbb94d9d2397b6" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6d852b27-1d95-4577-ac49-0d344a1f93d0"/>
     <xsd:import namespace="fef4af80-67d0-434d-aa7c-17eed15b0840"/>
     <xsd:import namespace="69e77a95-4add-417d-ac50-c09752e64638"/>
@@ -13192,7 +13183,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6d852b27-1d95-4577-ac49-0d344a1f93d0" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -13211,7 +13202,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -13276,7 +13267,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="27f97a9c-5df3-4967-8f8c-2479abf341ed" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="27f97a9c-5df3-4967-8f8c-2479abf341ed" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -13323,8 +13314,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -13413,16 +13404,25 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E49D155-2C11-4885-ACD3-E6D3BF89105E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2787CFFA-3460-4A04-BA0A-9FECDEAA6229}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2787CFFA-3460-4A04-BA0A-9FECDEAA6229}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B855CC39-79B7-471A-9581-96C02B6745EC}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB476E3C-1092-486A-9BFE-5C9EC71BF137}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E49D155-2C11-4885-ACD3-E6D3BF89105E}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>